<commit_message>
finished modules, minor cleanup
</commit_message>
<xml_diff>
--- a/AlternaCanvas/data/ui/metadata.xlsx
+++ b/AlternaCanvas/data/ui/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jauri/Dropbox/UCincinnati stuff/UI-course/course-data/ui/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c75d2b7f1f30a064/school/FALL22/USER INTERFACE/User-Interface-Design/AlternaCanvas/data/ui/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B94BAA4-0071-F940-84D8-472910167E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="26840" windowHeight="15940" xr2:uid="{65432498-6129-1143-9E4B-D4F785041594}"/>
+    <workbookView xWindow="-19965" yWindow="435" windowWidth="18120" windowHeight="16050" xr2:uid="{65432498-6129-1143-9E4B-D4F785041594}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -501,14 +501,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -825,19 +823,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{635C220F-C380-DA45-B9E2-275B5014ECFA}">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.33203125" customWidth="1"/>
+    <col min="1" max="1" width="39.375" customWidth="1"/>
     <col min="6" max="6" width="14.5" customWidth="1"/>
     <col min="7" max="7" width="13.5" customWidth="1"/>
-    <col min="9" max="9" width="22.6640625" customWidth="1"/>
+    <col min="9" max="9" width="22.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -869,7 +867,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -901,7 +899,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>29</v>
       </c>
@@ -933,7 +931,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -965,7 +963,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -997,7 +995,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1029,7 +1027,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>81</v>
       </c>
@@ -1061,7 +1059,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>31</v>
       </c>
@@ -1093,7 +1091,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1125,7 +1123,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1157,7 +1155,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1189,7 +1187,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>33</v>
       </c>
@@ -1218,39 +1216,39 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>131</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F13" s="6">
+      <c r="C13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="1">
         <v>44811</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="1">
         <v>44850</v>
       </c>
-      <c r="H13" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="I13" s="5" t="s">
+      <c r="H13" t="s">
+        <v>70</v>
+      </c>
+      <c r="I13" t="s">
         <v>132</v>
       </c>
-      <c r="J13" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1263,7 +1261,7 @@
       <c r="D14" t="s">
         <v>78</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14">
         <v>1</v>
       </c>
       <c r="F14" s="1">
@@ -1282,7 +1280,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>82</v>
       </c>
@@ -1295,7 +1293,7 @@
       <c r="D15" t="s">
         <v>78</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15">
         <v>1</v>
       </c>
       <c r="F15" s="1">
@@ -1314,7 +1312,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>106</v>
       </c>
@@ -1327,7 +1325,7 @@
       <c r="D16" t="s">
         <v>78</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16">
         <v>1</v>
       </c>
       <c r="F16" s="1">
@@ -1346,7 +1344,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>108</v>
       </c>
@@ -1359,7 +1357,7 @@
       <c r="D17" t="s">
         <v>78</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17">
         <v>1</v>
       </c>
       <c r="F17" s="1">
@@ -1378,7 +1376,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1391,7 +1389,7 @@
       <c r="D18" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18">
         <v>1</v>
       </c>
       <c r="F18" s="1">
@@ -1410,7 +1408,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>110</v>
       </c>
@@ -1423,7 +1421,7 @@
       <c r="D19" t="s">
         <v>78</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19">
         <v>1</v>
       </c>
       <c r="F19" s="1">
@@ -1442,7 +1440,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>83</v>
       </c>
@@ -1455,7 +1453,7 @@
       <c r="D20" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20">
         <v>10</v>
       </c>
       <c r="F20" s="1">
@@ -1474,7 +1472,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>84</v>
       </c>
@@ -1487,7 +1485,7 @@
       <c r="D21" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21">
         <v>10</v>
       </c>
       <c r="F21" s="1">
@@ -1506,7 +1504,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>34</v>
       </c>
@@ -1535,7 +1533,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -1548,7 +1546,7 @@
       <c r="D23" t="s">
         <v>78</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23">
         <v>1</v>
       </c>
       <c r="F23" s="1">
@@ -1564,7 +1562,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>85</v>
       </c>
@@ -1577,7 +1575,7 @@
       <c r="D24" t="s">
         <v>79</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24">
         <v>1</v>
       </c>
       <c r="F24" s="1">
@@ -1593,7 +1591,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>89</v>
       </c>
@@ -1606,7 +1604,7 @@
       <c r="D25" t="s">
         <v>78</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25">
         <v>1</v>
       </c>
       <c r="F25" s="1">
@@ -1622,7 +1620,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>113</v>
       </c>
@@ -1635,7 +1633,7 @@
       <c r="D26" t="s">
         <v>78</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26">
         <v>1</v>
       </c>
       <c r="F26" s="1">
@@ -1651,7 +1649,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -1664,7 +1662,7 @@
       <c r="D27" t="s">
         <v>78</v>
       </c>
-      <c r="E27" s="5">
+      <c r="E27">
         <v>1</v>
       </c>
       <c r="F27" s="1">
@@ -1680,7 +1678,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>92</v>
       </c>
@@ -1693,7 +1691,7 @@
       <c r="D28" t="s">
         <v>78</v>
       </c>
-      <c r="E28" s="5">
+      <c r="E28">
         <v>1</v>
       </c>
       <c r="F28" s="1">
@@ -1709,7 +1707,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>115</v>
       </c>
@@ -1722,7 +1720,7 @@
       <c r="D29" t="s">
         <v>78</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E29">
         <v>1</v>
       </c>
       <c r="F29" s="1">
@@ -1738,7 +1736,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -1751,7 +1749,7 @@
       <c r="D30" t="s">
         <v>78</v>
       </c>
-      <c r="E30" s="5">
+      <c r="E30">
         <v>1</v>
       </c>
       <c r="F30" s="1">
@@ -1767,7 +1765,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>116</v>
       </c>
@@ -1780,7 +1778,7 @@
       <c r="D31" t="s">
         <v>78</v>
       </c>
-      <c r="E31" s="5">
+      <c r="E31">
         <v>1</v>
       </c>
       <c r="F31" s="1">
@@ -1796,7 +1794,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>90</v>
       </c>
@@ -1809,7 +1807,7 @@
       <c r="D32" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="5">
+      <c r="E32">
         <v>10</v>
       </c>
       <c r="F32" s="1">
@@ -1828,7 +1826,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>35</v>
       </c>
@@ -1854,7 +1852,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -1867,7 +1865,7 @@
       <c r="D34" t="s">
         <v>78</v>
       </c>
-      <c r="E34" s="5">
+      <c r="E34">
         <v>1</v>
       </c>
       <c r="F34" s="1">
@@ -1883,7 +1881,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>94</v>
       </c>
@@ -1896,7 +1894,7 @@
       <c r="D35" t="s">
         <v>78</v>
       </c>
-      <c r="E35" s="5">
+      <c r="E35">
         <v>1</v>
       </c>
       <c r="F35" s="1">
@@ -1912,7 +1910,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>96</v>
       </c>
@@ -1941,7 +1939,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>118</v>
       </c>
@@ -1954,7 +1952,7 @@
       <c r="D37" t="s">
         <v>78</v>
       </c>
-      <c r="E37" s="5">
+      <c r="E37">
         <v>1</v>
       </c>
       <c r="F37" s="1">
@@ -1970,7 +1968,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>18</v>
       </c>
@@ -1983,7 +1981,7 @@
       <c r="D38" t="s">
         <v>78</v>
       </c>
-      <c r="E38" s="5">
+      <c r="E38">
         <v>1</v>
       </c>
       <c r="F38" s="1">
@@ -1999,7 +1997,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>98</v>
       </c>
@@ -2028,7 +2026,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>119</v>
       </c>
@@ -2041,7 +2039,7 @@
       <c r="D40" t="s">
         <v>78</v>
       </c>
-      <c r="E40" s="5">
+      <c r="E40">
         <v>1</v>
       </c>
       <c r="F40" s="1">
@@ -2057,7 +2055,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>19</v>
       </c>
@@ -2070,7 +2068,7 @@
       <c r="D41" t="s">
         <v>78</v>
       </c>
-      <c r="E41" s="5">
+      <c r="E41">
         <v>1</v>
       </c>
       <c r="F41" s="1">
@@ -2086,7 +2084,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>123</v>
       </c>
@@ -2099,7 +2097,7 @@
       <c r="D42" t="s">
         <v>78</v>
       </c>
-      <c r="E42" s="5">
+      <c r="E42">
         <v>1</v>
       </c>
       <c r="F42" s="1">
@@ -2115,7 +2113,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>121</v>
       </c>
@@ -2128,7 +2126,7 @@
       <c r="D43" t="s">
         <v>44</v>
       </c>
-      <c r="E43" s="5">
+      <c r="E43">
         <v>10</v>
       </c>
       <c r="F43" s="1">
@@ -2147,7 +2145,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>122</v>
       </c>
@@ -2160,7 +2158,7 @@
       <c r="D44" t="s">
         <v>44</v>
       </c>
-      <c r="E44" s="5">
+      <c r="E44">
         <v>10</v>
       </c>
       <c r="F44" s="1">
@@ -2176,7 +2174,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>39</v>
       </c>
@@ -2202,7 +2200,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>20</v>
       </c>
@@ -2215,7 +2213,7 @@
       <c r="D46" t="s">
         <v>78</v>
       </c>
-      <c r="E46" s="5">
+      <c r="E46">
         <v>1</v>
       </c>
       <c r="F46" s="1">
@@ -2231,7 +2229,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>123</v>
       </c>
@@ -2244,7 +2242,7 @@
       <c r="D47" t="s">
         <v>78</v>
       </c>
-      <c r="E47" s="5">
+      <c r="E47">
         <v>1</v>
       </c>
       <c r="F47" s="1">
@@ -2260,7 +2258,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>21</v>
       </c>
@@ -2273,7 +2271,7 @@
       <c r="D48" t="s">
         <v>78</v>
       </c>
-      <c r="E48" s="5">
+      <c r="E48">
         <v>1</v>
       </c>
       <c r="F48" s="1">
@@ -2289,7 +2287,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>127</v>
       </c>
@@ -2302,7 +2300,7 @@
       <c r="D49" t="s">
         <v>78</v>
       </c>
-      <c r="E49" s="5">
+      <c r="E49">
         <v>1</v>
       </c>
       <c r="F49" s="1">
@@ -2318,7 +2316,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>22</v>
       </c>
@@ -2331,7 +2329,7 @@
       <c r="D50" t="s">
         <v>78</v>
       </c>
-      <c r="E50" s="5">
+      <c r="E50">
         <v>1</v>
       </c>
       <c r="F50" s="1">
@@ -2347,7 +2345,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>129</v>
       </c>
@@ -2360,7 +2358,7 @@
       <c r="D51" t="s">
         <v>78</v>
       </c>
-      <c r="E51" s="5">
+      <c r="E51">
         <v>1</v>
       </c>
       <c r="F51" s="1">
@@ -2376,7 +2374,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="52" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>40</v>
       </c>
@@ -2402,7 +2400,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>23</v>
       </c>
@@ -2415,7 +2413,7 @@
       <c r="D53" t="s">
         <v>78</v>
       </c>
-      <c r="E53" s="5">
+      <c r="E53">
         <v>1</v>
       </c>
       <c r="F53" s="1">
@@ -2431,7 +2429,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>24</v>
       </c>
@@ -2444,7 +2442,7 @@
       <c r="D54" t="s">
         <v>78</v>
       </c>
-      <c r="E54" s="5">
+      <c r="E54">
         <v>1</v>
       </c>
       <c r="F54" s="1">
@@ -2460,7 +2458,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>25</v>
       </c>
@@ -2473,7 +2471,7 @@
       <c r="D55" t="s">
         <v>78</v>
       </c>
-      <c r="E55" s="5">
+      <c r="E55">
         <v>1</v>
       </c>
       <c r="F55" s="1">
@@ -2489,7 +2487,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>26</v>
       </c>
@@ -2502,7 +2500,7 @@
       <c r="D56" t="s">
         <v>78</v>
       </c>
-      <c r="E56" s="5">
+      <c r="E56">
         <v>1</v>
       </c>
       <c r="F56" s="1">
@@ -2518,7 +2516,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>69</v>
       </c>
@@ -2531,7 +2529,7 @@
       <c r="D57" t="s">
         <v>80</v>
       </c>
-      <c r="E57" s="5">
+      <c r="E57">
         <v>50</v>
       </c>
       <c r="F57" s="1">
@@ -2550,7 +2548,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>72</v>
       </c>
@@ -2563,7 +2561,7 @@
       <c r="D58" t="s">
         <v>80</v>
       </c>
-      <c r="E58" s="5">
+      <c r="E58">
         <v>40</v>
       </c>
       <c r="F58" s="1">

</xml_diff>